<commit_message>
Be compatible with MATLAB 2018
</commit_message>
<xml_diff>
--- a/doc/pollynet_output_results_info.xlsx
+++ b/doc/pollynet_output_results_info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="181">
   <si>
     <t>Filename</t>
   </si>
@@ -544,6 +544,24 @@
   </si>
   <si>
     <t>volume depolarization ratio at 532 nm</t>
+  </si>
+  <si>
+    <t>yyyy_mm_dd_ddd_polly_HH_MM_SS_target_classification.nc</t>
+  </si>
+  <si>
+    <t>2018_12_31_Mon_LACROS_06_00_01_target_classification.nc</t>
+  </si>
+  <si>
+    <t>target_classification</t>
+  </si>
+  <si>
+    <t>target classification</t>
+  </si>
+  <si>
+    <t>yyyy_mm_dd_ddd_polly_HH_MM_SS_WVMR_RH.nc</t>
+  </si>
+  <si>
+    <t>2018_12_31_Mon_LACROS_06_00_01_WVMR_RH.nc</t>
   </si>
 </sst>
 </file>
@@ -617,7 +635,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -655,6 +673,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -663,7 +718,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
@@ -687,6 +742,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -699,7 +755,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
@@ -984,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L97"/>
+  <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:L96"/>
+    <sheetView tabSelected="1" topLeftCell="B94" workbookViewId="0">
+      <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1038,10 +1114,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1076,8 +1152,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="4" t="s">
         <v>36</v>
       </c>
@@ -1110,8 +1186,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1144,8 +1220,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="4" t="s">
         <v>37</v>
       </c>
@@ -1178,8 +1254,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1212,8 +1288,8 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="4" t="s">
         <v>38</v>
       </c>
@@ -1246,8 +1322,8 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
@@ -1276,8 +1352,8 @@
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
@@ -1306,8 +1382,8 @@
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1338,8 +1414,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1368,8 +1444,8 @@
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="4" t="s">
         <v>15</v>
       </c>
@@ -1398,8 +1474,8 @@
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
@@ -1430,8 +1506,8 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="4" t="s">
         <v>17</v>
       </c>
@@ -1460,8 +1536,8 @@
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="4" t="s">
         <v>18</v>
       </c>
@@ -1490,8 +1566,8 @@
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
@@ -1522,8 +1598,8 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
@@ -1552,8 +1628,8 @@
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
@@ -1582,8 +1658,8 @@
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="4" t="s">
         <v>22</v>
       </c>
@@ -1612,8 +1688,8 @@
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="4" t="s">
         <v>23</v>
       </c>
@@ -1642,8 +1718,8 @@
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="4" t="s">
         <v>24</v>
       </c>
@@ -1672,8 +1748,8 @@
       <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1702,8 +1778,8 @@
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="4" t="s">
         <v>26</v>
       </c>
@@ -1732,8 +1808,8 @@
       <c r="L23" s="6"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="4" t="s">
         <v>27</v>
       </c>
@@ -1762,8 +1838,8 @@
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="4" t="s">
         <v>28</v>
       </c>
@@ -1792,8 +1868,8 @@
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="4" t="s">
         <v>70</v>
       </c>
@@ -1822,8 +1898,8 @@
       <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="4" t="s">
         <v>29</v>
       </c>
@@ -1852,8 +1928,8 @@
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="4" t="s">
         <v>30</v>
       </c>
@@ -1884,8 +1960,8 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="4" t="s">
         <v>31</v>
       </c>
@@ -1916,8 +1992,8 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="4" t="s">
         <v>32</v>
       </c>
@@ -1948,8 +2024,8 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="4" t="s">
         <v>33</v>
       </c>
@@ -1978,8 +2054,8 @@
       <c r="L31" s="6"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="4" t="s">
         <v>34</v>
       </c>
@@ -2008,8 +2084,8 @@
       <c r="L32" s="6"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="4" t="s">
         <v>35</v>
       </c>
@@ -2038,10 +2114,10 @@
       <c r="L33" s="6"/>
     </row>
     <row r="34" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="17" t="s">
         <v>76</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -2076,8 +2152,8 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
       <c r="C35" s="1" t="s">
         <v>36</v>
       </c>
@@ -2110,8 +2186,8 @@
       </c>
     </row>
     <row r="36" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
       <c r="C36" s="1" t="s">
         <v>10</v>
       </c>
@@ -2144,8 +2220,8 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="16"/>
-      <c r="B37" s="16"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
       <c r="C37" s="1" t="s">
         <v>37</v>
       </c>
@@ -2178,8 +2254,8 @@
       </c>
     </row>
     <row r="38" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="16"/>
-      <c r="B38" s="16"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
       <c r="C38" s="1" t="s">
         <v>9</v>
       </c>
@@ -2212,8 +2288,8 @@
       </c>
     </row>
     <row r="39" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
       <c r="C39" s="1" t="s">
         <v>78</v>
       </c>
@@ -2246,8 +2322,8 @@
       </c>
     </row>
     <row r="40" spans="1:12" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="16"/>
-      <c r="B40" s="16"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
       <c r="C40" s="1" t="s">
         <v>79</v>
       </c>
@@ -2278,8 +2354,8 @@
       <c r="L40" s="11"/>
     </row>
     <row r="41" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="16"/>
-      <c r="B41" s="16"/>
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
       <c r="C41" s="1" t="s">
         <v>80</v>
       </c>
@@ -2312,8 +2388,8 @@
       </c>
     </row>
     <row r="42" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="16"/>
-      <c r="B42" s="16"/>
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
       <c r="C42" s="1" t="s">
         <v>81</v>
       </c>
@@ -2344,8 +2420,8 @@
       <c r="L42" s="11"/>
     </row>
     <row r="43" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
       <c r="C43" s="1" t="s">
         <v>82</v>
       </c>
@@ -2376,8 +2452,8 @@
       <c r="L43" s="11"/>
     </row>
     <row r="44" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="16"/>
-      <c r="B44" s="16"/>
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
       <c r="C44" s="1" t="s">
         <v>83</v>
       </c>
@@ -2410,8 +2486,8 @@
       </c>
     </row>
     <row r="45" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="16"/>
-      <c r="B45" s="16"/>
+      <c r="A45" s="17"/>
+      <c r="B45" s="17"/>
       <c r="C45" s="1" t="s">
         <v>84</v>
       </c>
@@ -2442,8 +2518,8 @@
       <c r="L45" s="11"/>
     </row>
     <row r="46" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="16"/>
-      <c r="B46" s="16"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
       <c r="C46" s="1" t="s">
         <v>85</v>
       </c>
@@ -2474,8 +2550,8 @@
       <c r="L46" s="11"/>
     </row>
     <row r="47" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="16"/>
-      <c r="B47" s="16"/>
+      <c r="A47" s="17"/>
+      <c r="B47" s="17"/>
       <c r="C47" s="1" t="s">
         <v>86</v>
       </c>
@@ -2508,8 +2584,8 @@
       </c>
     </row>
     <row r="48" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="16"/>
-      <c r="B48" s="16"/>
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
       <c r="C48" s="1" t="s">
         <v>121</v>
       </c>
@@ -2540,8 +2616,8 @@
       <c r="L48" s="11"/>
     </row>
     <row r="49" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="16"/>
-      <c r="B49" s="16"/>
+      <c r="A49" s="17"/>
+      <c r="B49" s="17"/>
       <c r="C49" s="1" t="s">
         <v>87</v>
       </c>
@@ -2572,8 +2648,8 @@
       <c r="L49" s="11"/>
     </row>
     <row r="50" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="16"/>
-      <c r="B50" s="16"/>
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
       <c r="C50" s="1" t="s">
         <v>88</v>
       </c>
@@ -2606,8 +2682,8 @@
       </c>
     </row>
     <row r="51" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="16"/>
-      <c r="B51" s="16"/>
+      <c r="A51" s="17"/>
+      <c r="B51" s="17"/>
       <c r="C51" s="1" t="s">
         <v>89</v>
       </c>
@@ -2638,8 +2714,8 @@
       <c r="L51" s="11"/>
     </row>
     <row r="52" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="16"/>
-      <c r="B52" s="16"/>
+      <c r="A52" s="17"/>
+      <c r="B52" s="17"/>
       <c r="C52" s="1" t="s">
         <v>90</v>
       </c>
@@ -2670,8 +2746,8 @@
       <c r="L52" s="11"/>
     </row>
     <row r="53" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="16"/>
-      <c r="B53" s="16"/>
+      <c r="A53" s="17"/>
+      <c r="B53" s="17"/>
       <c r="C53" s="1" t="s">
         <v>91</v>
       </c>
@@ -2704,8 +2780,8 @@
       </c>
     </row>
     <row r="54" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="16"/>
-      <c r="B54" s="16"/>
+      <c r="A54" s="17"/>
+      <c r="B54" s="17"/>
       <c r="C54" s="1" t="s">
         <v>92</v>
       </c>
@@ -2736,8 +2812,8 @@
       <c r="L54" s="11"/>
     </row>
     <row r="55" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="16"/>
-      <c r="B55" s="16"/>
+      <c r="A55" s="17"/>
+      <c r="B55" s="17"/>
       <c r="C55" s="1" t="s">
         <v>93</v>
       </c>
@@ -2766,8 +2842,8 @@
       <c r="L55" s="11"/>
     </row>
     <row r="56" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="16"/>
-      <c r="B56" s="16"/>
+      <c r="A56" s="17"/>
+      <c r="B56" s="17"/>
       <c r="C56" s="1" t="s">
         <v>94</v>
       </c>
@@ -2796,8 +2872,8 @@
       <c r="L56" s="11"/>
     </row>
     <row r="57" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="16"/>
-      <c r="B57" s="16"/>
+      <c r="A57" s="17"/>
+      <c r="B57" s="17"/>
       <c r="C57" s="1" t="s">
         <v>95</v>
       </c>
@@ -2826,8 +2902,8 @@
       </c>
     </row>
     <row r="58" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="16"/>
-      <c r="B58" s="16"/>
+      <c r="A58" s="17"/>
+      <c r="B58" s="17"/>
       <c r="C58" s="1" t="s">
         <v>96</v>
       </c>
@@ -2856,8 +2932,8 @@
       <c r="L58" s="11"/>
     </row>
     <row r="59" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="16"/>
-      <c r="B59" s="16"/>
+      <c r="A59" s="17"/>
+      <c r="B59" s="17"/>
       <c r="C59" s="1" t="s">
         <v>97</v>
       </c>
@@ -2884,8 +2960,8 @@
       <c r="L59" s="11"/>
     </row>
     <row r="60" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="16"/>
-      <c r="B60" s="16"/>
+      <c r="A60" s="17"/>
+      <c r="B60" s="17"/>
       <c r="C60" s="1" t="s">
         <v>98</v>
       </c>
@@ -2916,8 +2992,8 @@
       </c>
     </row>
     <row r="61" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="16"/>
-      <c r="B61" s="16"/>
+      <c r="A61" s="17"/>
+      <c r="B61" s="17"/>
       <c r="C61" s="1" t="s">
         <v>99</v>
       </c>
@@ -2944,8 +3020,8 @@
       <c r="L61" s="11"/>
     </row>
     <row r="62" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="16"/>
-      <c r="B62" s="16"/>
+      <c r="A62" s="17"/>
+      <c r="B62" s="17"/>
       <c r="C62" s="1" t="s">
         <v>100</v>
       </c>
@@ -2974,8 +3050,8 @@
       </c>
     </row>
     <row r="63" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="16"/>
-      <c r="B63" s="16"/>
+      <c r="A63" s="17"/>
+      <c r="B63" s="17"/>
       <c r="C63" s="1" t="s">
         <v>101</v>
       </c>
@@ -3006,8 +3082,8 @@
       <c r="L63" s="11"/>
     </row>
     <row r="64" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="16"/>
-      <c r="B64" s="16"/>
+      <c r="A64" s="17"/>
+      <c r="B64" s="17"/>
       <c r="C64" s="1" t="s">
         <v>102</v>
       </c>
@@ -3036,8 +3112,8 @@
       <c r="L64" s="11"/>
     </row>
     <row r="65" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="16"/>
-      <c r="B65" s="16"/>
+      <c r="A65" s="17"/>
+      <c r="B65" s="17"/>
       <c r="C65" s="1" t="s">
         <v>103</v>
       </c>
@@ -3070,8 +3146,8 @@
       </c>
     </row>
     <row r="66" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="16"/>
-      <c r="B66" s="16"/>
+      <c r="A66" s="17"/>
+      <c r="B66" s="17"/>
       <c r="C66" s="1" t="s">
         <v>104</v>
       </c>
@@ -3104,8 +3180,8 @@
       </c>
     </row>
     <row r="67" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="16"/>
-      <c r="B67" s="16"/>
+      <c r="A67" s="17"/>
+      <c r="B67" s="17"/>
       <c r="C67" s="1" t="s">
         <v>105</v>
       </c>
@@ -3136,8 +3212,8 @@
       <c r="L67" s="11"/>
     </row>
     <row r="68" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="16"/>
-      <c r="B68" s="16"/>
+      <c r="A68" s="17"/>
+      <c r="B68" s="17"/>
       <c r="C68" s="1" t="s">
         <v>106</v>
       </c>
@@ -3170,8 +3246,8 @@
       </c>
     </row>
     <row r="69" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="16"/>
-      <c r="B69" s="16"/>
+      <c r="A69" s="17"/>
+      <c r="B69" s="17"/>
       <c r="C69" s="1" t="s">
         <v>107</v>
       </c>
@@ -3202,8 +3278,8 @@
       <c r="L69" s="11"/>
     </row>
     <row r="70" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="16"/>
-      <c r="B70" s="16"/>
+      <c r="A70" s="17"/>
+      <c r="B70" s="17"/>
       <c r="C70" s="1" t="s">
         <v>108</v>
       </c>
@@ -3234,8 +3310,8 @@
       <c r="L70" s="11"/>
     </row>
     <row r="71" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="16"/>
-      <c r="B71" s="16"/>
+      <c r="A71" s="17"/>
+      <c r="B71" s="17"/>
       <c r="C71" s="1" t="s">
         <v>109</v>
       </c>
@@ -3268,8 +3344,8 @@
       </c>
     </row>
     <row r="72" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="16"/>
-      <c r="B72" s="16"/>
+      <c r="A72" s="17"/>
+      <c r="B72" s="17"/>
       <c r="C72" s="1" t="s">
         <v>110</v>
       </c>
@@ -3300,10 +3376,10 @@
       <c r="L72" s="11"/>
     </row>
     <row r="73" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="14" t="s">
+      <c r="A73" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B73" s="15" t="s">
         <v>151</v>
       </c>
       <c r="C73" s="8" t="s">
@@ -3338,8 +3414,8 @@
       </c>
     </row>
     <row r="74" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="14"/>
-      <c r="B74" s="14"/>
+      <c r="A74" s="15"/>
+      <c r="B74" s="15"/>
       <c r="C74" s="8" t="s">
         <v>36</v>
       </c>
@@ -3372,8 +3448,8 @@
       </c>
     </row>
     <row r="75" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="14"/>
-      <c r="B75" s="14"/>
+      <c r="A75" s="15"/>
+      <c r="B75" s="15"/>
       <c r="C75" s="8" t="s">
         <v>10</v>
       </c>
@@ -3406,8 +3482,8 @@
       </c>
     </row>
     <row r="76" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="14"/>
-      <c r="B76" s="14"/>
+      <c r="A76" s="15"/>
+      <c r="B76" s="15"/>
       <c r="C76" s="8" t="s">
         <v>38</v>
       </c>
@@ -3440,8 +3516,8 @@
       </c>
     </row>
     <row r="77" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="14"/>
-      <c r="B77" s="14"/>
+      <c r="A77" s="15"/>
+      <c r="B77" s="15"/>
       <c r="C77" s="8" t="s">
         <v>78</v>
       </c>
@@ -3474,8 +3550,8 @@
       </c>
     </row>
     <row r="78" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="14"/>
-      <c r="B78" s="14"/>
+      <c r="A78" s="15"/>
+      <c r="B78" s="15"/>
       <c r="C78" s="8" t="s">
         <v>153</v>
       </c>
@@ -3506,8 +3582,8 @@
       <c r="L78" s="12"/>
     </row>
     <row r="79" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="14"/>
-      <c r="B79" s="14"/>
+      <c r="A79" s="15"/>
+      <c r="B79" s="15"/>
       <c r="C79" s="8" t="s">
         <v>155</v>
       </c>
@@ -3540,8 +3616,8 @@
       </c>
     </row>
     <row r="80" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="14"/>
-      <c r="B80" s="14"/>
+      <c r="A80" s="15"/>
+      <c r="B80" s="15"/>
       <c r="C80" s="8" t="s">
         <v>157</v>
       </c>
@@ -3572,10 +3648,10 @@
       <c r="L80" s="12"/>
     </row>
     <row r="81" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="13" t="s">
+      <c r="A81" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="B81" s="13" t="s">
+      <c r="B81" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C81" s="9" t="s">
@@ -3587,31 +3663,31 @@
       <c r="E81" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F81" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G81" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H81" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I81" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J81" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K81" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L81" s="17" t="s">
+      <c r="F81" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G81" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H81" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I81" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J81" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K81" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L81" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="13"/>
-      <c r="B82" s="13"/>
+      <c r="A82" s="14"/>
+      <c r="B82" s="14"/>
       <c r="C82" s="9" t="s">
         <v>36</v>
       </c>
@@ -3621,31 +3697,31 @@
       <c r="E82" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F82" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G82" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H82" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I82" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J82" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K82" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L82" s="17" t="s">
+      <c r="F82" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G82" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H82" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I82" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J82" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K82" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L82" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="13"/>
-      <c r="B83" s="13"/>
+      <c r="A83" s="14"/>
+      <c r="B83" s="14"/>
       <c r="C83" s="9" t="s">
         <v>10</v>
       </c>
@@ -3655,31 +3731,31 @@
       <c r="E83" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F83" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G83" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H83" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I83" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J83" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K83" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L83" s="17" t="s">
+      <c r="F83" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G83" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H83" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I83" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J83" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K83" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L83" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="13"/>
-      <c r="B84" s="13"/>
+      <c r="A84" s="14"/>
+      <c r="B84" s="14"/>
       <c r="C84" s="9" t="s">
         <v>38</v>
       </c>
@@ -3689,31 +3765,31 @@
       <c r="E84" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F84" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G84" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H84" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I84" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J84" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K84" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L84" s="17" t="s">
+      <c r="F84" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G84" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H84" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I84" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J84" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K84" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L84" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="13"/>
-      <c r="B85" s="13"/>
+      <c r="A85" s="14"/>
+      <c r="B85" s="14"/>
       <c r="C85" s="9" t="s">
         <v>78</v>
       </c>
@@ -3723,31 +3799,31 @@
       <c r="E85" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F85" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G85" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H85" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I85" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J85" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K85" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L85" s="17" t="s">
+      <c r="F85" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G85" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H85" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I85" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J85" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K85" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L85" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="13"/>
-      <c r="B86" s="13"/>
+      <c r="A86" s="14"/>
+      <c r="B86" s="14"/>
       <c r="C86" s="9" t="s">
         <v>161</v>
       </c>
@@ -3757,31 +3833,31 @@
       <c r="E86" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="F86" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G86" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H86" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I86" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J86" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K86" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L86" s="17" t="s">
+      <c r="F86" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G86" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H86" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I86" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J86" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K86" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L86" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="13"/>
-      <c r="B87" s="13"/>
+      <c r="A87" s="14"/>
+      <c r="B87" s="14"/>
       <c r="C87" s="9" t="s">
         <v>163</v>
       </c>
@@ -3791,29 +3867,29 @@
       <c r="E87" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="F87" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G87" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H87" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I87" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J87" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K87" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L87" s="17"/>
+      <c r="F87" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G87" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H87" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I87" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J87" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K87" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L87" s="13"/>
     </row>
     <row r="88" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="13"/>
-      <c r="B88" s="13"/>
+      <c r="A88" s="14"/>
+      <c r="B88" s="14"/>
       <c r="C88" s="9" t="s">
         <v>165</v>
       </c>
@@ -3821,29 +3897,29 @@
         <v>166</v>
       </c>
       <c r="E88" s="10"/>
-      <c r="F88" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G88" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H88" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I88" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J88" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K88" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L88" s="17"/>
+      <c r="F88" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G88" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H88" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I88" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J88" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K88" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L88" s="13"/>
     </row>
     <row r="89" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="13"/>
-      <c r="B89" s="13"/>
+      <c r="A89" s="14"/>
+      <c r="B89" s="14"/>
       <c r="C89" s="9" t="s">
         <v>167</v>
       </c>
@@ -3851,31 +3927,31 @@
         <v>168</v>
       </c>
       <c r="E89" s="10"/>
-      <c r="F89" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G89" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H89" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I89" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J89" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K89" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L89" s="17"/>
+      <c r="F89" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G89" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H89" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I89" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J89" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K89" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L89" s="13"/>
     </row>
     <row r="90" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="14" t="s">
+      <c r="A90" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="B90" s="14" t="s">
+      <c r="B90" s="15" t="s">
         <v>169</v>
       </c>
       <c r="C90" s="8" t="s">
@@ -3910,8 +3986,8 @@
       </c>
     </row>
     <row r="91" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="14"/>
-      <c r="B91" s="14"/>
+      <c r="A91" s="15"/>
+      <c r="B91" s="15"/>
       <c r="C91" s="8" t="s">
         <v>36</v>
       </c>
@@ -3944,8 +4020,8 @@
       </c>
     </row>
     <row r="92" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="14"/>
-      <c r="B92" s="14"/>
+      <c r="A92" s="15"/>
+      <c r="B92" s="15"/>
       <c r="C92" s="8" t="s">
         <v>10</v>
       </c>
@@ -3978,8 +4054,8 @@
       </c>
     </row>
     <row r="93" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="14"/>
-      <c r="B93" s="14"/>
+      <c r="A93" s="15"/>
+      <c r="B93" s="15"/>
       <c r="C93" s="8" t="s">
         <v>38</v>
       </c>
@@ -4012,8 +4088,8 @@
       </c>
     </row>
     <row r="94" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="14"/>
-      <c r="B94" s="14"/>
+      <c r="A94" s="15"/>
+      <c r="B94" s="15"/>
       <c r="C94" s="8" t="s">
         <v>78</v>
       </c>
@@ -4042,8 +4118,8 @@
       <c r="L94" s="12"/>
     </row>
     <row r="95" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="14"/>
-      <c r="B95" s="14"/>
+      <c r="A95" s="15"/>
+      <c r="B95" s="15"/>
       <c r="C95" s="8" t="s">
         <v>171</v>
       </c>
@@ -4074,8 +4150,8 @@
       </c>
     </row>
     <row r="96" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="14"/>
-      <c r="B96" s="14"/>
+      <c r="A96" s="15"/>
+      <c r="B96" s="15"/>
       <c r="C96" s="8" t="s">
         <v>173</v>
       </c>
@@ -4097,9 +4173,421 @@
       <c r="K96" s="12"/>
       <c r="L96" s="12"/>
     </row>
-    <row r="97" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="97" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A97" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="B97" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F97" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G97" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H97" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I97" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J97" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K97" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L97" s="11"/>
+    </row>
+    <row r="98" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="17"/>
+      <c r="B98" s="20"/>
+      <c r="C98" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F98" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G98" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H98" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I98" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J98" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K98" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L98" s="11"/>
+    </row>
+    <row r="99" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="17"/>
+      <c r="B99" s="20"/>
+      <c r="C99" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F99" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G99" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H99" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I99" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J99" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K99" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L99" s="11"/>
+    </row>
+    <row r="100" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A100" s="17"/>
+      <c r="B100" s="20"/>
+      <c r="C100" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F100" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G100" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H100" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I100" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J100" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K100" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L100" s="11"/>
+    </row>
+    <row r="101" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="17"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F101" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G101" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H101" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I101" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J101" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K101" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L101" s="11"/>
+    </row>
+    <row r="102" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A102" s="17"/>
+      <c r="B102" s="21"/>
+      <c r="C102" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E102" s="1"/>
+      <c r="F102" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G102" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H102" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I102" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J102" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K102" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L102" s="11"/>
+    </row>
+    <row r="103" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A103" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="B103" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F103" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G103" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H103" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I103" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J103" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K103" s="13"/>
+      <c r="L103" s="13"/>
+    </row>
+    <row r="104" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A104" s="23"/>
+      <c r="B104" s="23"/>
+      <c r="C104" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D104" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F104" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G104" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H104" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I104" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J104" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K104" s="13"/>
+      <c r="L104" s="13"/>
+    </row>
+    <row r="105" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A105" s="23"/>
+      <c r="B105" s="23"/>
+      <c r="C105" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D105" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F105" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G105" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H105" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I105" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J105" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K105" s="13"/>
+      <c r="L105" s="13"/>
+    </row>
+    <row r="106" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="23"/>
+      <c r="B106" s="23"/>
+      <c r="C106" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D106" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F106" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G106" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H106" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I106" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J106" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K106" s="13"/>
+      <c r="L106" s="13"/>
+    </row>
+    <row r="107" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="23"/>
+      <c r="B107" s="23"/>
+      <c r="C107" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F107" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G107" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H107" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I107" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J107" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K107" s="13"/>
+      <c r="L107" s="13"/>
+    </row>
+    <row r="108" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A108" s="23"/>
+      <c r="B108" s="23"/>
+      <c r="C108" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D108" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E108" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F108" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G108" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H108" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I108" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J108" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K108" s="13"/>
+      <c r="L108" s="13"/>
+    </row>
+    <row r="109" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="24"/>
+      <c r="B109" s="24"/>
+      <c r="C109" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D109" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F109" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G109" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H109" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I109" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J109" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K109" s="13"/>
+      <c r="L109" s="13"/>
+    </row>
+    <row r="110" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
+    <mergeCell ref="B97:B102"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A103:A109"/>
+    <mergeCell ref="B103:B109"/>
     <mergeCell ref="A81:A89"/>
     <mergeCell ref="B81:B89"/>
     <mergeCell ref="A90:A96"/>

</xml_diff>